<commit_message>
Assignment 4 final push checkout cart adding user details finish implement TestNg
</commit_message>
<xml_diff>
--- a/src/main/java/dataFile/UsersDetails.xlsx
+++ b/src/main/java/dataFile/UsersDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ndhurandher\intellij-workspace\Selenium_Assignment_4_5\src\main\java\dataFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3853E77-43C5-4E8F-93A2-00684A7EE107}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CDE156-EA5D-402E-89F6-2BC9AA839586}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>username</t>
   </si>
@@ -46,6 +46,24 @@
   </si>
   <si>
     <t>performance_glitch_user</t>
+  </si>
+  <si>
+    <t>first name</t>
+  </si>
+  <si>
+    <t>last name</t>
+  </si>
+  <si>
+    <t>pin code</t>
+  </si>
+  <si>
+    <t>fhjag</t>
+  </si>
+  <si>
+    <t>hfajh</t>
+  </si>
+  <si>
+    <t>gfhaf</t>
   </si>
 </sst>
 </file>
@@ -363,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -375,47 +393,93 @@
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Assignment 4 final push checkout cart adding user details finish implement TestNg, log4j, Parallel execution, report creator
</commit_message>
<xml_diff>
--- a/src/main/java/dataFile/UsersDetails.xlsx
+++ b/src/main/java/dataFile/UsersDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ndhurandher\intellij-workspace\Selenium_Assignment_4_5\src\main\java\dataFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CDE156-EA5D-402E-89F6-2BC9AA839586}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98794185-4D92-472E-B8F8-81696C989B89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>username</t>
   </si>
@@ -57,13 +57,40 @@
     <t>pin code</t>
   </si>
   <si>
-    <t>fhjag</t>
-  </si>
-  <si>
-    <t>hfajh</t>
-  </si>
-  <si>
-    <t>gfhaf</t>
+    <t>Aman</t>
+  </si>
+  <si>
+    <t>Sahil</t>
+  </si>
+  <si>
+    <t>Rohit</t>
+  </si>
+  <si>
+    <t>Abhishek</t>
+  </si>
+  <si>
+    <t>Bansal</t>
+  </si>
+  <si>
+    <t>Awasthi</t>
+  </si>
+  <si>
+    <t>Dharam</t>
+  </si>
+  <si>
+    <t>Chaudhary</t>
+  </si>
+  <si>
+    <t>A12345</t>
+  </si>
+  <si>
+    <t>A12346</t>
+  </si>
+  <si>
+    <t>A12347</t>
+  </si>
+  <si>
+    <t>A12348</t>
   </si>
 </sst>
 </file>
@@ -384,7 +411,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -421,10 +448,10 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -435,13 +462,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -452,13 +479,13 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -469,13 +496,13 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>